<commit_message>
Extended grid search all working
</commit_message>
<xml_diff>
--- a/Notebooks/Model_Comparisons_v1.xlsx
+++ b/Notebooks/Model_Comparisons_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stuartgow/GitHub/EEG_ML_Pipeline/Notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC32BB39-62B3-484E-9044-55CE83335D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEAF3B39-63EA-9A46-A8B0-7EBF6884A0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="800" windowWidth="29320" windowHeight="26020" xr2:uid="{4EF99E70-5403-6B47-9FEC-848AE0CD045D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="108">
   <si>
     <t>Model</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>Channels</t>
-  </si>
-  <si>
-    <t>Aperiodic</t>
   </si>
   <si>
     <t>Models Evaluation</t>
@@ -143,9 +140,6 @@
     <t>Slightly better on FN</t>
   </si>
   <si>
-    <t>Very good TP but sveral FN</t>
-  </si>
-  <si>
     <t>?? MCC</t>
   </si>
   <si>
@@ -366,6 +360,9 @@
   </si>
   <si>
     <t>Add subject reduces the quality of predictions</t>
+  </si>
+  <si>
+    <t>Very good TP but several FN</t>
   </si>
 </sst>
 </file>
@@ -559,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -618,16 +615,31 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -637,29 +649,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1003,7 +993,7 @@
   <dimension ref="A1:U144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="D6" sqref="D6:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1024,7 +1014,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -1042,46 +1032,46 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="26" t="s">
+      <c r="C4" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="D4" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="E4" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="H4" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="I4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="31" t="s">
         <v>5</v>
       </c>
       <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="25"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="32"/>
       <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:13" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -1093,7 +1083,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="E6" s="2">
         <v>5.5E-2</v>
@@ -1115,7 +1105,7 @@
       </c>
       <c r="K6" s="7"/>
       <c r="M6" s="18" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -1127,7 +1117,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="E7" s="2">
         <v>3.8E-3</v>
@@ -1149,7 +1139,7 @@
       </c>
       <c r="K7" s="7"/>
       <c r="M7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -1161,7 +1151,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="E8" s="4">
         <v>2.2000000000000001E-3</v>
@@ -1183,7 +1173,7 @@
       </c>
       <c r="K8" s="7"/>
       <c r="M8" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -1201,13 +1191,13 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="M11" s="34" t="s">
-        <v>67</v>
+        <v>15</v>
+      </c>
+      <c r="M11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -1216,16 +1206,16 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -1233,10 +1223,10 @@
         <v>6</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1244,10 +1234,10 @@
         <v>7</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
@@ -1255,10 +1245,10 @@
         <v>8</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
@@ -1276,46 +1266,46 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="26" t="s">
+      <c r="C21" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="D21" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="30" t="s">
+      <c r="E21" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G21" s="31" t="s">
+      <c r="G21" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="H21" s="30" t="s">
+      <c r="H21" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="I21" s="30" t="s">
+      <c r="I21" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="J21" s="24" t="s">
+      <c r="J21" s="31" t="s">
         <v>5</v>
       </c>
       <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="25"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="32"/>
       <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -1324,10 +1314,10 @@
         <v>6</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E23" s="2">
         <v>3.6200000000000003E-2</v>
@@ -1349,7 +1339,7 @@
       </c>
       <c r="K23" s="7"/>
       <c r="M23" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -1358,10 +1348,10 @@
         <v>7</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E24" s="2">
         <v>2.9999999999999997E-4</v>
@@ -1389,10 +1379,10 @@
         <v>8</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E25" s="4">
         <v>8.0000000000000004E-4</v>
@@ -1414,10 +1404,10 @@
       </c>
       <c r="K25" s="7"/>
       <c r="M25" s="20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N25" s="21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O25" s="21"/>
       <c r="P25" s="21"/>
@@ -1437,13 +1427,13 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
-      </c>
-      <c r="M28" s="34" t="s">
-        <v>68</v>
+        <v>15</v>
+      </c>
+      <c r="M28" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
@@ -1452,16 +1442,16 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
@@ -1472,7 +1462,7 @@
         <v>7.4</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
@@ -1483,7 +1473,7 @@
         <v>0.4</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
@@ -1494,7 +1484,7 @@
         <v>2.59</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
@@ -1512,49 +1502,49 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D37" s="26" t="s">
+      <c r="C37" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E37" s="26" t="s">
+      <c r="D37" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F37" s="30" t="s">
+      <c r="E37" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G37" s="31" t="s">
+      <c r="G37" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="H37" s="30" t="s">
+      <c r="H37" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="I37" s="30" t="s">
+      <c r="I37" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="J37" s="24" t="s">
+      <c r="J37" s="31" t="s">
         <v>5</v>
       </c>
       <c r="K37" s="6"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="6"/>
-      <c r="B38" s="29"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
-      <c r="J38" s="25"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="32"/>
       <c r="K38" s="6"/>
       <c r="N38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -1566,7 +1556,7 @@
         <v>10</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E39" s="2">
         <v>3.2000000000000001E-2</v>
@@ -1583,15 +1573,15 @@
       <c r="I39" s="17">
         <v>0.2727</v>
       </c>
-      <c r="J39" s="35">
+      <c r="J39" s="5">
         <v>0.312</v>
       </c>
       <c r="K39" s="7"/>
-      <c r="M39" s="37" t="s">
-        <v>88</v>
+      <c r="M39" s="25" t="s">
+        <v>86</v>
       </c>
       <c r="N39" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O39" s="21"/>
       <c r="P39" s="21"/>
@@ -1607,7 +1597,7 @@
         <v>10</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E40" s="2">
         <v>4.0000000000000002E-4</v>
@@ -1615,7 +1605,7 @@
       <c r="F40" s="2">
         <v>0.73680000000000001</v>
       </c>
-      <c r="G40" s="35">
+      <c r="G40" s="5">
         <v>0.7</v>
       </c>
       <c r="H40" s="2">
@@ -1629,7 +1619,7 @@
       </c>
       <c r="K40" s="7"/>
       <c r="M40" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -1641,7 +1631,7 @@
         <v>10</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E41" s="4">
         <v>1.06E-2</v>
@@ -1662,11 +1652,11 @@
         <v>0.2823</v>
       </c>
       <c r="K41" s="7"/>
-      <c r="M41" s="38" t="s">
-        <v>92</v>
+      <c r="M41" s="26" t="s">
+        <v>90</v>
       </c>
       <c r="N41" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
@@ -1684,13 +1674,13 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D44" t="s">
-        <v>16</v>
-      </c>
-      <c r="M44" s="34" t="s">
-        <v>86</v>
+        <v>15</v>
+      </c>
+      <c r="M44" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
@@ -1699,16 +1689,16 @@
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
@@ -1719,7 +1709,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
@@ -1730,7 +1720,7 @@
         <v>5.67</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
@@ -1741,7 +1731,7 @@
         <v>5.76</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.2">
@@ -1759,46 +1749,46 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="6"/>
-      <c r="B53" s="28" t="s">
+      <c r="B53" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C53" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D53" s="26" t="s">
+      <c r="C53" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E53" s="26" t="s">
+      <c r="D53" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F53" s="30" t="s">
+      <c r="E53" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G53" s="31" t="s">
+      <c r="G53" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="H53" s="30" t="s">
+      <c r="H53" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="I53" s="30" t="s">
+      <c r="I53" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="J53" s="24" t="s">
+      <c r="J53" s="31" t="s">
         <v>5</v>
       </c>
       <c r="K53" s="6"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" s="6"/>
-      <c r="B54" s="29"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="27"/>
-      <c r="G54" s="32"/>
-      <c r="H54" s="27"/>
-      <c r="I54" s="27"/>
-      <c r="J54" s="25"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="30"/>
+      <c r="G54" s="28"/>
+      <c r="H54" s="30"/>
+      <c r="I54" s="30"/>
+      <c r="J54" s="32"/>
       <c r="K54" s="6"/>
     </row>
     <row r="55" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -1807,10 +1797,10 @@
         <v>6</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E55" s="2">
         <v>3.0099999999999998E-2</v>
@@ -1832,13 +1822,13 @@
       </c>
       <c r="K55" s="7"/>
       <c r="M55" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="N55" t="s">
+        <v>97</v>
+      </c>
+      <c r="O55" t="s">
         <v>99</v>
-      </c>
-      <c r="O55" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -1847,10 +1837,10 @@
         <v>7</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E56" s="2">
         <v>4.0000000000000002E-4</v>
@@ -1858,7 +1848,7 @@
       <c r="F56" s="2">
         <v>0.57889999999999997</v>
       </c>
-      <c r="G56" s="35">
+      <c r="G56" s="5">
         <v>0.73329999999999995</v>
       </c>
       <c r="H56" s="2">
@@ -1867,15 +1857,15 @@
       <c r="I56" s="5">
         <v>0.63639999999999997</v>
       </c>
-      <c r="J56" s="35">
+      <c r="J56" s="5">
         <v>0.20749999999999999</v>
       </c>
       <c r="K56" s="7"/>
       <c r="M56" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="N56" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O56" s="19"/>
       <c r="P56" s="19"/>
@@ -1888,10 +1878,10 @@
         <v>8</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E57" s="4">
         <v>6.9999999999999999E-4</v>
@@ -1913,10 +1903,10 @@
       </c>
       <c r="K57" s="7"/>
       <c r="M57" s="19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N57" s="21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="O57" s="21"/>
       <c r="P57" s="21"/>
@@ -1936,18 +1926,18 @@
       <c r="J58" s="6"/>
       <c r="K58" s="6"/>
       <c r="N58" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D60" t="s">
-        <v>16</v>
-      </c>
-      <c r="M60" s="34" t="s">
-        <v>96</v>
+        <v>15</v>
+      </c>
+      <c r="M60" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.2">
@@ -1956,16 +1946,16 @@
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.2">
@@ -1976,7 +1966,7 @@
         <v>8.16</v>
       </c>
       <c r="D64" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
@@ -1987,7 +1977,7 @@
         <v>0.39</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
@@ -1998,7 +1988,7 @@
         <v>2.92</v>
       </c>
       <c r="D66" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
@@ -2016,46 +2006,46 @@
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="6"/>
-      <c r="B70" s="28" t="s">
+      <c r="B70" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C70" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D70" s="26" t="s">
+      <c r="C70" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E70" s="26" t="s">
+      <c r="D70" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F70" s="30" t="s">
+      <c r="E70" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F70" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G70" s="31" t="s">
+      <c r="G70" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="H70" s="30" t="s">
+      <c r="H70" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="I70" s="30" t="s">
+      <c r="I70" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="J70" s="24" t="s">
+      <c r="J70" s="31" t="s">
         <v>5</v>
       </c>
       <c r="K70" s="6"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="6"/>
-      <c r="B71" s="29"/>
-      <c r="C71" s="27"/>
-      <c r="D71" s="27"/>
-      <c r="E71" s="27"/>
-      <c r="F71" s="27"/>
-      <c r="G71" s="32"/>
-      <c r="H71" s="27"/>
-      <c r="I71" s="27"/>
-      <c r="J71" s="25"/>
+      <c r="B71" s="34"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="30"/>
+      <c r="F71" s="30"/>
+      <c r="G71" s="28"/>
+      <c r="H71" s="30"/>
+      <c r="I71" s="30"/>
+      <c r="J71" s="32"/>
       <c r="K71" s="6"/>
     </row>
     <row r="72" spans="1:17" ht="23" customHeight="1" x14ac:dyDescent="0.2">
@@ -2067,7 +2057,7 @@
         <v>10</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E72" s="2">
         <v>3.1199999999999999E-2</v>
@@ -2089,7 +2079,7 @@
       </c>
       <c r="K72" s="7"/>
       <c r="M72" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="1:17" ht="23" customHeight="1" x14ac:dyDescent="0.2">
@@ -2101,7 +2091,7 @@
         <v>10</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E73" s="2">
         <v>3.8E-3</v>
@@ -2123,7 +2113,7 @@
       </c>
       <c r="K73" s="7"/>
       <c r="M73" s="19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="74" spans="1:17" ht="23" customHeight="1" x14ac:dyDescent="0.2">
@@ -2135,7 +2125,7 @@
         <v>10</v>
       </c>
       <c r="D74" s="23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E74" s="4">
         <v>2.3999999999999998E-3</v>
@@ -2157,7 +2147,7 @@
       </c>
       <c r="K74" s="7"/>
       <c r="M74" s="19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
@@ -2175,16 +2165,16 @@
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D77" t="s">
-        <v>16</v>
-      </c>
-      <c r="M77" s="34" t="s">
-        <v>69</v>
+        <v>15</v>
+      </c>
+      <c r="M77" t="s">
+        <v>67</v>
       </c>
       <c r="N77" s="19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
@@ -2193,10 +2183,10 @@
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N78" s="21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O78" s="21"/>
       <c r="P78" s="21"/>
@@ -2204,11 +2194,11 @@
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.2">
@@ -2219,7 +2209,7 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="D81" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.2">
@@ -2230,7 +2220,7 @@
         <v>68.930000000000007</v>
       </c>
       <c r="D82" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.2">
@@ -2241,7 +2231,7 @@
         <v>23.6</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.2">
@@ -2259,46 +2249,46 @@
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A87" s="6"/>
-      <c r="B87" s="28" t="s">
+      <c r="B87" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C87" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D87" s="26" t="s">
+      <c r="C87" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E87" s="26" t="s">
+      <c r="D87" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F87" s="30" t="s">
+      <c r="E87" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F87" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G87" s="31" t="s">
+      <c r="G87" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="H87" s="30" t="s">
+      <c r="H87" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="I87" s="30" t="s">
+      <c r="I87" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="J87" s="24" t="s">
+      <c r="J87" s="31" t="s">
         <v>5</v>
       </c>
       <c r="K87" s="6"/>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A88" s="6"/>
-      <c r="B88" s="29"/>
-      <c r="C88" s="27"/>
-      <c r="D88" s="27"/>
-      <c r="E88" s="27"/>
-      <c r="F88" s="27"/>
-      <c r="G88" s="32"/>
-      <c r="H88" s="27"/>
-      <c r="I88" s="27"/>
-      <c r="J88" s="25"/>
+      <c r="B88" s="34"/>
+      <c r="C88" s="30"/>
+      <c r="D88" s="30"/>
+      <c r="E88" s="30"/>
+      <c r="F88" s="30"/>
+      <c r="G88" s="28"/>
+      <c r="H88" s="30"/>
+      <c r="I88" s="30"/>
+      <c r="J88" s="32"/>
       <c r="K88" s="6"/>
     </row>
     <row r="89" spans="1:21" ht="23" customHeight="1" x14ac:dyDescent="0.2">
@@ -2307,10 +2297,10 @@
         <v>6</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E89" s="2">
         <v>2.7900000000000001E-2</v>
@@ -2332,16 +2322,16 @@
       </c>
       <c r="K89" s="7"/>
       <c r="M89" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="N89" s="21" t="s">
         <v>73</v>
-      </c>
-      <c r="N89" s="21" t="s">
-        <v>75</v>
       </c>
       <c r="O89" s="21"/>
       <c r="P89" s="21"/>
       <c r="Q89" s="21"/>
       <c r="S89" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="T89" s="21"/>
       <c r="U89" s="21"/>
@@ -2352,18 +2342,18 @@
         <v>7</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E90" s="2">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="F90" s="35">
+      <c r="F90" s="5">
         <v>0.73680000000000001</v>
       </c>
-      <c r="G90" s="35">
+      <c r="G90" s="5">
         <v>0.63639999999999997</v>
       </c>
       <c r="H90" s="2">
@@ -2377,7 +2367,7 @@
       </c>
       <c r="K90" s="7"/>
       <c r="M90" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="91" spans="1:21" ht="23" customHeight="1" x14ac:dyDescent="0.2">
@@ -2386,10 +2376,10 @@
         <v>8</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D91" s="23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E91" s="4">
         <v>6.9999999999999999E-4</v>
@@ -2411,17 +2401,17 @@
       </c>
       <c r="K91" s="7"/>
       <c r="M91" s="20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="N91" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O91" s="21"/>
       <c r="P91" s="21"/>
       <c r="Q91" s="21"/>
       <c r="R91" s="21"/>
       <c r="S91" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.2">
@@ -2437,7 +2427,7 @@
       <c r="J92" s="6"/>
       <c r="K92" s="6"/>
       <c r="N92" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="O92" s="21"/>
       <c r="P92" s="21"/>
@@ -2446,10 +2436,10 @@
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D94" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.2">
@@ -2457,26 +2447,20 @@
         <v>9</v>
       </c>
       <c r="C95" s="1"/>
-      <c r="D95" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="E95" s="34"/>
-      <c r="F95" s="34"/>
-      <c r="G95" s="34"/>
-      <c r="H95" s="34"/>
-      <c r="I95" s="34"/>
-      <c r="J95" s="34"/>
+      <c r="D95" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="M95" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
@@ -2487,7 +2471,7 @@
         <v>7.53</v>
       </c>
       <c r="D98" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
@@ -2498,7 +2482,7 @@
         <v>3.9</v>
       </c>
       <c r="D99" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
@@ -2509,7 +2493,7 @@
         <v>3.55</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
@@ -2527,46 +2511,46 @@
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" s="6"/>
-      <c r="B104" s="28" t="s">
+      <c r="B104" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C104" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D104" s="26" t="s">
+      <c r="C104" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E104" s="26" t="s">
+      <c r="D104" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F104" s="30" t="s">
+      <c r="E104" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F104" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G104" s="31" t="s">
+      <c r="G104" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="H104" s="30" t="s">
+      <c r="H104" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="I104" s="30" t="s">
+      <c r="I104" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="J104" s="24" t="s">
+      <c r="J104" s="31" t="s">
         <v>5</v>
       </c>
       <c r="K104" s="6"/>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" s="6"/>
-      <c r="B105" s="29"/>
-      <c r="C105" s="27"/>
-      <c r="D105" s="27"/>
-      <c r="E105" s="27"/>
-      <c r="F105" s="27"/>
-      <c r="G105" s="32"/>
-      <c r="H105" s="27"/>
-      <c r="I105" s="27"/>
-      <c r="J105" s="25"/>
+      <c r="B105" s="34"/>
+      <c r="C105" s="30"/>
+      <c r="D105" s="30"/>
+      <c r="E105" s="30"/>
+      <c r="F105" s="30"/>
+      <c r="G105" s="28"/>
+      <c r="H105" s="30"/>
+      <c r="I105" s="30"/>
+      <c r="J105" s="32"/>
       <c r="K105" s="6"/>
     </row>
     <row r="106" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2578,7 +2562,7 @@
         <v>10</v>
       </c>
       <c r="D106" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E106" s="2">
         <v>2.8899999999999999E-2</v>
@@ -2600,7 +2584,7 @@
       </c>
       <c r="K106" s="7"/>
       <c r="M106" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="107" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2612,7 +2596,7 @@
         <v>10</v>
       </c>
       <c r="D107" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E107" s="5">
         <v>2.8E-3</v>
@@ -2634,10 +2618,10 @@
       </c>
       <c r="K107" s="7"/>
       <c r="M107" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N107" s="21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O107" s="21"/>
       <c r="P107" s="21"/>
@@ -2652,7 +2636,7 @@
         <v>10</v>
       </c>
       <c r="D108" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E108" s="4">
         <v>1.1000000000000001E-3</v>
@@ -2674,7 +2658,7 @@
       </c>
       <c r="K108" s="7"/>
       <c r="M108" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
@@ -2692,16 +2676,16 @@
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D111" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M111" t="s">
+        <v>44</v>
+      </c>
+      <c r="N111" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="N111" s="21" t="s">
-        <v>48</v>
       </c>
       <c r="O111" s="21"/>
       <c r="P111" s="21"/>
@@ -2713,16 +2697,16 @@
       </c>
       <c r="C112" s="1"/>
       <c r="D112" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C113" s="1"/>
       <c r="D113" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
@@ -2733,7 +2717,7 @@
         <v>7.79</v>
       </c>
       <c r="D115" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.2">
@@ -2744,7 +2728,7 @@
         <v>61.61</v>
       </c>
       <c r="D116" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
@@ -2755,7 +2739,7 @@
         <v>20.56</v>
       </c>
       <c r="D117" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
@@ -2773,46 +2757,46 @@
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" s="6"/>
-      <c r="B120" s="28" t="s">
+      <c r="B120" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C120" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D120" s="26" t="s">
+      <c r="C120" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E120" s="26" t="s">
+      <c r="D120" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F120" s="30" t="s">
+      <c r="E120" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F120" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G120" s="31" t="s">
+      <c r="G120" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="H120" s="30" t="s">
+      <c r="H120" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="I120" s="30" t="s">
+      <c r="I120" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="J120" s="24" t="s">
+      <c r="J120" s="31" t="s">
         <v>5</v>
       </c>
       <c r="K120" s="6"/>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" s="6"/>
-      <c r="B121" s="29"/>
-      <c r="C121" s="27"/>
-      <c r="D121" s="27"/>
-      <c r="E121" s="27"/>
-      <c r="F121" s="27"/>
-      <c r="G121" s="32"/>
-      <c r="H121" s="27"/>
-      <c r="I121" s="27"/>
-      <c r="J121" s="25"/>
+      <c r="B121" s="34"/>
+      <c r="C121" s="30"/>
+      <c r="D121" s="30"/>
+      <c r="E121" s="30"/>
+      <c r="F121" s="30"/>
+      <c r="G121" s="28"/>
+      <c r="H121" s="30"/>
+      <c r="I121" s="30"/>
+      <c r="J121" s="32"/>
       <c r="K121" s="6"/>
     </row>
     <row r="122" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2821,10 +2805,10 @@
         <v>6</v>
       </c>
       <c r="C122" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D122" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E122" s="2">
         <v>4.6199999999999998E-2</v>
@@ -2846,10 +2830,10 @@
       </c>
       <c r="K122" s="7"/>
       <c r="M122" s="20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N122" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="123" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2858,10 +2842,10 @@
         <v>7</v>
       </c>
       <c r="C123" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D123" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E123" s="5">
         <v>1.8E-3</v>
@@ -2875,7 +2859,7 @@
       <c r="H123" s="3">
         <v>0.84209999999999996</v>
       </c>
-      <c r="I123" s="35">
+      <c r="I123" s="5">
         <v>0.72729999999999995</v>
       </c>
       <c r="J123" s="3">
@@ -2883,7 +2867,7 @@
       </c>
       <c r="K123" s="7"/>
       <c r="M123" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="124" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2892,10 +2876,10 @@
         <v>8</v>
       </c>
       <c r="C124" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D124" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E124" s="4">
         <v>2.3E-3</v>
@@ -2909,15 +2893,15 @@
       <c r="H124" s="4">
         <v>0.78049999999999997</v>
       </c>
-      <c r="I124" s="36">
+      <c r="I124" s="24">
         <v>0.45450000000000002</v>
       </c>
-      <c r="J124" s="36">
+      <c r="J124" s="24">
         <v>0.32329999999999998</v>
       </c>
       <c r="K124" s="7"/>
       <c r="M124" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.2">
@@ -2935,13 +2919,13 @@
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D127" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M127" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.2">
@@ -2949,22 +2933,17 @@
         <v>9</v>
       </c>
       <c r="C128" s="1"/>
-      <c r="D128" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="E128" s="34"/>
-      <c r="F128" s="34"/>
-      <c r="G128" s="34"/>
-      <c r="H128" s="34"/>
-      <c r="I128" s="34"/>
+      <c r="D128" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="129" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C129" s="1"/>
       <c r="D129" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="131" spans="2:8" x14ac:dyDescent="0.2">
@@ -2975,7 +2954,7 @@
         <v>7.95</v>
       </c>
       <c r="D131" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="132" spans="2:8" x14ac:dyDescent="0.2">
@@ -2986,7 +2965,7 @@
         <v>3.68</v>
       </c>
       <c r="D132" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="133" spans="2:8" x14ac:dyDescent="0.2">
@@ -2997,12 +2976,12 @@
         <v>3.56</v>
       </c>
       <c r="D133" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="137" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B137" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C137" s="21"/>
       <c r="D137" s="21"/>
@@ -3013,48 +2992,58 @@
     </row>
     <row r="141" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="142" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="143" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="144" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="J37:J38"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="H53:H54"/>
-    <mergeCell ref="I53:I54"/>
-    <mergeCell ref="J53:J54"/>
-    <mergeCell ref="H120:H121"/>
-    <mergeCell ref="I120:I121"/>
-    <mergeCell ref="J120:J121"/>
-    <mergeCell ref="B120:B121"/>
-    <mergeCell ref="C120:C121"/>
-    <mergeCell ref="D120:D121"/>
-    <mergeCell ref="E120:E121"/>
-    <mergeCell ref="F120:F121"/>
-    <mergeCell ref="G120:G121"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="E104:E105"/>
+    <mergeCell ref="F104:F105"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="G70:G71"/>
+    <mergeCell ref="H70:H71"/>
+    <mergeCell ref="I70:I71"/>
+    <mergeCell ref="J70:J71"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
     <mergeCell ref="G104:G105"/>
     <mergeCell ref="H104:H105"/>
     <mergeCell ref="I104:I105"/>
@@ -3071,40 +3060,30 @@
     <mergeCell ref="B104:B105"/>
     <mergeCell ref="C104:C105"/>
     <mergeCell ref="D104:D105"/>
-    <mergeCell ref="E104:E105"/>
-    <mergeCell ref="F104:F105"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="G70:G71"/>
-    <mergeCell ref="H70:H71"/>
-    <mergeCell ref="I70:I71"/>
-    <mergeCell ref="J70:J71"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="H120:H121"/>
+    <mergeCell ref="I120:I121"/>
+    <mergeCell ref="J120:J121"/>
+    <mergeCell ref="B120:B121"/>
+    <mergeCell ref="C120:C121"/>
+    <mergeCell ref="D120:D121"/>
+    <mergeCell ref="E120:E121"/>
+    <mergeCell ref="F120:F121"/>
+    <mergeCell ref="G120:G121"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="J37:J38"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="H53:H54"/>
+    <mergeCell ref="I53:I54"/>
+    <mergeCell ref="J53:J54"/>
     <mergeCell ref="E37:E38"/>
     <mergeCell ref="F37:F38"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="H21:H22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
eval to df saves
</commit_message>
<xml_diff>
--- a/Notebooks/Model_Comparisons_v1.xlsx
+++ b/Notebooks/Model_Comparisons_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stuartgow/GitHub/EEG_ML_Pipeline/Notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB657F3-D957-0C45-87DB-0AE7F140EEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148F0203-6E6F-6B49-8161-AF59B50F81CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="800" windowWidth="29320" windowHeight="26020" xr2:uid="{4EF99E70-5403-6B47-9FEC-848AE0CD045D}"/>
+    <workbookView xWindow="29140" yWindow="620" windowWidth="29320" windowHeight="26020" xr2:uid="{4EF99E70-5403-6B47-9FEC-848AE0CD045D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -630,16 +630,23 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -649,15 +656,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -999,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87625442-3BD6-D848-B867-F3AC6454CEE0}">
   <dimension ref="A1:U144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O94" sqref="O94"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1039,46 +1039,46 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="33" t="s">
+      <c r="I4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="27" t="s">
+      <c r="J4" s="32" t="s">
         <v>5</v>
       </c>
       <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="28"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="33"/>
       <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:13" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -1273,46 +1273,46 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G21" s="34" t="s">
+      <c r="G21" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H21" s="33" t="s">
+      <c r="H21" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I21" s="33" t="s">
+      <c r="I21" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J21" s="27" t="s">
+      <c r="J21" s="32" t="s">
         <v>5</v>
       </c>
       <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="28"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="33"/>
       <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -1509,46 +1509,46 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
-      <c r="B37" s="31" t="s">
+      <c r="B37" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="29" t="s">
+      <c r="C37" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D37" s="29" t="s">
+      <c r="D37" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="29" t="s">
+      <c r="E37" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F37" s="33" t="s">
+      <c r="F37" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G37" s="34" t="s">
+      <c r="G37" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H37" s="33" t="s">
+      <c r="H37" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I37" s="33" t="s">
+      <c r="I37" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J37" s="27" t="s">
+      <c r="J37" s="32" t="s">
         <v>5</v>
       </c>
       <c r="K37" s="6"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="6"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="35"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="28"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="33"/>
       <c r="K38" s="6"/>
       <c r="N38" t="s">
         <v>92</v>
@@ -1756,46 +1756,46 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="6"/>
-      <c r="B53" s="31" t="s">
+      <c r="B53" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C53" s="29" t="s">
+      <c r="C53" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D53" s="29" t="s">
+      <c r="D53" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E53" s="29" t="s">
+      <c r="E53" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F53" s="33" t="s">
+      <c r="F53" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G53" s="34" t="s">
+      <c r="G53" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H53" s="33" t="s">
+      <c r="H53" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I53" s="33" t="s">
+      <c r="I53" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J53" s="27" t="s">
+      <c r="J53" s="32" t="s">
         <v>5</v>
       </c>
       <c r="K53" s="6"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" s="6"/>
-      <c r="B54" s="32"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="30"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="30"/>
-      <c r="I54" s="30"/>
-      <c r="J54" s="28"/>
+      <c r="B54" s="35"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="29"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="31"/>
+      <c r="J54" s="33"/>
       <c r="K54" s="6"/>
     </row>
     <row r="55" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2013,46 +2013,46 @@
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="6"/>
-      <c r="B70" s="31" t="s">
+      <c r="B70" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C70" s="29" t="s">
+      <c r="C70" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D70" s="29" t="s">
+      <c r="D70" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E70" s="29" t="s">
+      <c r="E70" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F70" s="33" t="s">
+      <c r="F70" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G70" s="34" t="s">
+      <c r="G70" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H70" s="33" t="s">
+      <c r="H70" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I70" s="33" t="s">
+      <c r="I70" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J70" s="27" t="s">
+      <c r="J70" s="32" t="s">
         <v>5</v>
       </c>
       <c r="K70" s="6"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="6"/>
-      <c r="B71" s="32"/>
-      <c r="C71" s="30"/>
-      <c r="D71" s="30"/>
-      <c r="E71" s="30"/>
-      <c r="F71" s="30"/>
-      <c r="G71" s="35"/>
-      <c r="H71" s="30"/>
-      <c r="I71" s="30"/>
-      <c r="J71" s="28"/>
+      <c r="B71" s="35"/>
+      <c r="C71" s="31"/>
+      <c r="D71" s="31"/>
+      <c r="E71" s="31"/>
+      <c r="F71" s="31"/>
+      <c r="G71" s="29"/>
+      <c r="H71" s="31"/>
+      <c r="I71" s="31"/>
+      <c r="J71" s="33"/>
       <c r="K71" s="6"/>
     </row>
     <row r="72" spans="1:17" ht="23" customHeight="1" x14ac:dyDescent="0.2">
@@ -2256,46 +2256,46 @@
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A87" s="6"/>
-      <c r="B87" s="31" t="s">
+      <c r="B87" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C87" s="29" t="s">
+      <c r="C87" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D87" s="29" t="s">
+      <c r="D87" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E87" s="29" t="s">
+      <c r="E87" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F87" s="33" t="s">
+      <c r="F87" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G87" s="34" t="s">
+      <c r="G87" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H87" s="33" t="s">
+      <c r="H87" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I87" s="33" t="s">
+      <c r="I87" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J87" s="27" t="s">
+      <c r="J87" s="32" t="s">
         <v>5</v>
       </c>
       <c r="K87" s="6"/>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A88" s="6"/>
-      <c r="B88" s="32"/>
-      <c r="C88" s="30"/>
-      <c r="D88" s="30"/>
-      <c r="E88" s="30"/>
-      <c r="F88" s="30"/>
-      <c r="G88" s="35"/>
-      <c r="H88" s="30"/>
-      <c r="I88" s="30"/>
-      <c r="J88" s="28"/>
+      <c r="B88" s="35"/>
+      <c r="C88" s="31"/>
+      <c r="D88" s="31"/>
+      <c r="E88" s="31"/>
+      <c r="F88" s="31"/>
+      <c r="G88" s="29"/>
+      <c r="H88" s="31"/>
+      <c r="I88" s="31"/>
+      <c r="J88" s="33"/>
       <c r="K88" s="6"/>
     </row>
     <row r="89" spans="1:21" ht="23" customHeight="1" x14ac:dyDescent="0.2">
@@ -2457,7 +2457,7 @@
       <c r="D95" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="M95" s="36" t="s">
+      <c r="M95" s="27" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2518,46 +2518,46 @@
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" s="6"/>
-      <c r="B104" s="31" t="s">
+      <c r="B104" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C104" s="29" t="s">
+      <c r="C104" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D104" s="29" t="s">
+      <c r="D104" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E104" s="29" t="s">
+      <c r="E104" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F104" s="33" t="s">
+      <c r="F104" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G104" s="34" t="s">
+      <c r="G104" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H104" s="33" t="s">
+      <c r="H104" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I104" s="33" t="s">
+      <c r="I104" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J104" s="27" t="s">
+      <c r="J104" s="32" t="s">
         <v>5</v>
       </c>
       <c r="K104" s="6"/>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" s="6"/>
-      <c r="B105" s="32"/>
-      <c r="C105" s="30"/>
-      <c r="D105" s="30"/>
-      <c r="E105" s="30"/>
-      <c r="F105" s="30"/>
-      <c r="G105" s="35"/>
-      <c r="H105" s="30"/>
-      <c r="I105" s="30"/>
-      <c r="J105" s="28"/>
+      <c r="B105" s="35"/>
+      <c r="C105" s="31"/>
+      <c r="D105" s="31"/>
+      <c r="E105" s="31"/>
+      <c r="F105" s="31"/>
+      <c r="G105" s="29"/>
+      <c r="H105" s="31"/>
+      <c r="I105" s="31"/>
+      <c r="J105" s="33"/>
       <c r="K105" s="6"/>
     </row>
     <row r="106" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2764,46 +2764,46 @@
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" s="6"/>
-      <c r="B120" s="31" t="s">
+      <c r="B120" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C120" s="29" t="s">
+      <c r="C120" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D120" s="29" t="s">
+      <c r="D120" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E120" s="29" t="s">
+      <c r="E120" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F120" s="33" t="s">
+      <c r="F120" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G120" s="34" t="s">
+      <c r="G120" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H120" s="33" t="s">
+      <c r="H120" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I120" s="33" t="s">
+      <c r="I120" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J120" s="27" t="s">
+      <c r="J120" s="32" t="s">
         <v>5</v>
       </c>
       <c r="K120" s="6"/>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" s="6"/>
-      <c r="B121" s="32"/>
-      <c r="C121" s="30"/>
-      <c r="D121" s="30"/>
-      <c r="E121" s="30"/>
-      <c r="F121" s="30"/>
-      <c r="G121" s="35"/>
-      <c r="H121" s="30"/>
-      <c r="I121" s="30"/>
-      <c r="J121" s="28"/>
+      <c r="B121" s="35"/>
+      <c r="C121" s="31"/>
+      <c r="D121" s="31"/>
+      <c r="E121" s="31"/>
+      <c r="F121" s="31"/>
+      <c r="G121" s="29"/>
+      <c r="H121" s="31"/>
+      <c r="I121" s="31"/>
+      <c r="J121" s="33"/>
       <c r="K121" s="6"/>
     </row>
     <row r="122" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3019,30 +3019,38 @@
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="J37:J38"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="H53:H54"/>
-    <mergeCell ref="I53:I54"/>
-    <mergeCell ref="J53:J54"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="H120:H121"/>
-    <mergeCell ref="I120:I121"/>
-    <mergeCell ref="J120:J121"/>
-    <mergeCell ref="B120:B121"/>
-    <mergeCell ref="C120:C121"/>
-    <mergeCell ref="D120:D121"/>
-    <mergeCell ref="E120:E121"/>
-    <mergeCell ref="F120:F121"/>
-    <mergeCell ref="G120:G121"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="E104:E105"/>
+    <mergeCell ref="F104:F105"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="G70:G71"/>
+    <mergeCell ref="H70:H71"/>
+    <mergeCell ref="I70:I71"/>
+    <mergeCell ref="J70:J71"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
     <mergeCell ref="G104:G105"/>
     <mergeCell ref="H104:H105"/>
     <mergeCell ref="I104:I105"/>
@@ -3059,38 +3067,30 @@
     <mergeCell ref="B104:B105"/>
     <mergeCell ref="C104:C105"/>
     <mergeCell ref="D104:D105"/>
-    <mergeCell ref="E104:E105"/>
-    <mergeCell ref="F104:F105"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="G70:G71"/>
-    <mergeCell ref="H70:H71"/>
-    <mergeCell ref="I70:I71"/>
-    <mergeCell ref="J70:J71"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="H120:H121"/>
+    <mergeCell ref="I120:I121"/>
+    <mergeCell ref="J120:J121"/>
+    <mergeCell ref="B120:B121"/>
+    <mergeCell ref="C120:C121"/>
+    <mergeCell ref="D120:D121"/>
+    <mergeCell ref="E120:E121"/>
+    <mergeCell ref="F120:F121"/>
+    <mergeCell ref="G120:G121"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="J37:J38"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="H53:H54"/>
+    <mergeCell ref="I53:I54"/>
+    <mergeCell ref="J53:J54"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>